<commit_message>
Get daily reddit data: Tue Aug 20 08:10:20 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_25.xlsx
+++ b/data/2024_08_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C476"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2981 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1ewq28x</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how to remove residue nail glue from press on nails? </t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewq28x/how_to_remove_residue_nail_glue_from_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1ewpeb2</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Brat summer anyone?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/how70ikusrjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1ewo1gn</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seche Vite: why you be like this? </t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewo1gn/seche_vite_why_you_be_like_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1ewoutz</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>These were my natural nails 2 days ago. I chopped them all off today.</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewoutz</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1ewopx5</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Can't believe these are press ons. I love them!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewopx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1ewonxe</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>As a male, should I show my toes in public or just keep them hidden in socks and shoes? I'd love to hear some honest thoughts on guys with painted toes</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewonxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1ewon9z</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Obsessed with these Chainsaw Man nails</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewon9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1ewo9wr</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Damaged Nails Fix?</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewo9wr/damaged_nails_fix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1ewo4bc</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Cadillaquer-Lavender (Reflective)</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewo4bc</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1ewnpzm</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I haven't done my nails in a while, but the color changing ones based on temperature are my favorite! </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fh0hky6x8rjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1ewnmyl</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Delicate manicure</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kar44lb38rjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1ewncj7</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Cat eye nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewncj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1ewn2e8</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>any clear nail polishes tha doesnt peel off easily?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewn2e8/any_clear_nail_polishes_tha_doesnt_peel_off_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1ewl7r8</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxqstersjqjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1ewm6uw</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Am i better off just learning?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewm6uw/am_i_better_off_just_learning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1ewlpq1</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Showing off our nails</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oncrvg9hoqjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1ewkqwg</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Products </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewkqwg/products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1ewkl2l</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My recent fave lately. Pearly/milky nails. </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4psn4i4beqjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1ewkhql</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails my friend did :) </t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewkhql</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1ewixjg</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Small nail wand? </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewixjg/small_nail_wand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1ewhv9z</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome dust on gel? </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewhv9z/chrome_dust_on_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1ewhv4m</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4th time doing Gel X </t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewhv4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1ewicvd</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Which one??</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewicvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1ewjmkx</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pale nail beds </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewjmkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1ewjwsz</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink coquette set </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4sdrnpk8qjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1ewjktm</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>I will always come back to bubble bath</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cy2rxoq5qjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1ewjdjf</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue again </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewjdjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1ewjdea</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In my chrome era </t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx5pk66y3qjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1ewj79k</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌸🌸🌸 uñas muy delicadas ! </t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u11db1g2qjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1ewj53j</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Que les parece estas cutículas ?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79mtxumx1qjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1ewirg6</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Neon Butterflies</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewirg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1ewiooh</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>💚🏁</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewiooh</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1ewimrx</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Tips on Ombré Gradient Nails</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aq2mudakxpjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1ewhfba</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>what do you think? i love them! 💕✨🐮</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf37tdhqnpjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1ewhb6c</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Can you use DND, Kokoist and Nail Thoughts together?</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewhb6c/can_you_use_dnd_kokoist_and_nail_thoughts_together/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1ewh05g</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today black marble effect </t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewh05g</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1ewguf8</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love getting something new after getting something I didn’t like lol </t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qk1yx6e1jpjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1ewgb94</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>What should you call this nail shape?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjwzjbulepjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1ewg4ud</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>These press ons are EVERYTHING💕</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewg4ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1ewg3xn</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrocvmcycpjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1ewg0ln</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>I love this color</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2t73ogd7cpjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1ewfu8f</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>About two months of nail growth</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74nxgbhuapjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1ewfi2k</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Too soon for spooky nails?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0xl7iw78pjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1ewe71t</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>My nail tech is amazing!</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewe71t</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1ewdsbi</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">manicure done for a wedding. What do you think? </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bg0qeymlvojd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1ewdo54</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1j5ghx1ruojd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1ewdbcr</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Teal ombre with hearts 💙</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmm5sc6trojd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1ewc8uc</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">these came out pretty cute☺️ </t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nm4vscn5kojd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1ewc82i</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Constructive criticism please</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewc82i</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1ewb0gf</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone use Le Manoir Gelcare polish with Amazon LED lamp? </t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewb0gf/anyone_use_le_manoir_gelcare_polish_with_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1ewat1s</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>I had to do short gem free nails 😢 I think the magnetic polish saved these</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewat1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1ewap40</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>First time doing duck nails</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewap40</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1ew9wen</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel form? Advice needed. </t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ew9wen/gel_form_advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1ew9zh6</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Fast Drying/Long Lasting?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ew9zh6/fast_dryinglong_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1ew9r4f</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>New Set</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w37kvhdv2ojd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1ew9ocn</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>I’m completely new to nails so forgive me if this is a stupid question regarding press on nails</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ew9ocn/im_completely_new_to_nails_so_forgive_me_if_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1ew9nn3</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Galaxy toes! </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sdjv9r762ojd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1ew9mry</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Alloya from Taiwan</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opmpoxbf1ojd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1ew9j93</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Longest set I have ever done for a client 🤭👀</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew9j93</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1ew9j34</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looks a little “Easter” but I wanted something light and dainty. </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/reji8a791ojd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1ew9g8n</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Bridesmaid set</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew9g8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1ew9b5o</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Simply light pink</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0ge7s1pznjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1ew98q7</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Painted my nails for the kitties at the shelter I work at</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew98q7</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1ew8vsl</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>My best manicure</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mab4mpumwnjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1ew8uul</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Structured Manicure Gels</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ew8uul/structured_manicure_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1ew8lji</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Today’s set</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r771adclunjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1ew8756</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">jelly + glitter ✨️ </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3os6dicqrnjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1ew802d</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good matte top coat? </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpdrjjgaqnjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1ew7u86</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My middle acrylic came off it’s been 2 and a half weeks </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew7u86</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1ew2don</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Shifty blue/purple with an accent nail</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hlat8v5ulmjd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1evyfd6</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Ombre and practicing</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1evyfd6/ombre_and_practicing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1ew6sdc</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Gradient red-pink coffin shape + chrome powder</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew6sdc</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1ew6hvh</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Is it bad to use acetone if I have a crack like this ?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dptgggjfnjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1ew6fk9</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Cinnamoroll Polygel Nails I did on my right hand!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew6fk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1ew62o5</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel mani I did on myself </t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew62o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1ew5ybx</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail always splits—help! </t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi76coqnbnjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1ew567t</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been awhile 🖤 </t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzco9wc66njd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1ew4s47</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Set I did last night for a friend</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew4s47</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1ew4m04</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Card Captor Sakura Press-Ons</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j3qta9a2njd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1ew4ied</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love this mani </t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jocn61qk1njd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1ew453l</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recent sets as a beginner nail artist— all regular polish! Swipe for super cursed pose </t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew453l</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1ew4012</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Russian mani on my shorties!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew4012</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1ew3whm</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Want to get my nails done for holiday - help! </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ew3whm/want_to_get_my_nails_done_for_holiday_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1ew2u8f</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcf8w6pdpmjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1ew2rn4</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>My mermaid nails 🧜🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o755scouomjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1ew1us1</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>It's been 2 weeks. Some nails are lifted already. Should I take these off or get a fill in?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nu1vajvhmjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1ew1gg6</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>brown nails</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s150gopqemjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1ew1ez1</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>My nails this week! I love it 🩷</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rjkzu3neemjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1ew1bfn</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>New length (need advice)</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew1bfn</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1ew0zoa</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>My nails need care</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uhgbhd1bmjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1ew0kj4</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">August and July nails 🥰 (now pink) </t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew0kj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1ew01sx</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Ariel character art 🧜🏻‍♀️🦞</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y2p1spy2mjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1evyrry</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Just got my naaaails 💅</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0zdkdrzpljd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1evy7to</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Colour changes to stretch time between infills</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1evy7to/colour_changes_to_stretch_time_between_infills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1evy38x</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Quinceanera set  </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1evy38x</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1evxagi</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>my simple nails</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9wkjhhb8ljd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1ewoxny</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Took the nail oiling seriously</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewoxny</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1ewo4m0</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Cadillaquer-Lavender (Reflective)</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewo4m0</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1ewnl0m</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Small but mighty</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ad3t9xmi7rjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1ewn62a</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>What are some cute cooler toned colours for a fall velvet manicure?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewn62a/what_are_some_cute_cooler_toned_colours_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1ewkjpj</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One Foot In The Ground - Paint it Pretty </t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewkjpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1ewjfqy</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>The purple Essie Hard to Resist is literally purple shampoo for your nails! 💜</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8emd9si4qjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1ewjctr</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In my chrome era </t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxy9zq0t3qjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1ewj7so</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>How long before gel x nails can be removed?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewj7so/how_long_before_gel_x_nails_can_be_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1ewiz4i</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Recommendations for tip shape?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewiz4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1ewiq1x</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Neon Butterflies for the RL Discord Monthly Challenge</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewiq1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1ewgt6z</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Lord help me I've been suffering with nails lately apparently I just don't want nails anymore I want decals gel polish mostly removed but now what the fuck??</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uo8hc5zripjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1ewgq8r</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>How my color blind husband sees my nail polish pretties (Protanopia)</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewgq8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1ewgokj</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>What do we think about these little guys from Prism UK? (base coat and top coat) Has anyone here tried them?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0viqcplphpjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1ewg6e3</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Made my first ILNP order, I'm obsessed with these!</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewg6e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1ewaddt</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Biogel Nail Help</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewaddt/biogel_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1ew6ivt</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Dupe for my favorite discontinued polish?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew6ivt</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1ewgmj1</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Indie Sales?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewgmj1/indie_sales/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1evsc86</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Just a bit excited about my nails</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abfkvxtiljjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1ewgknl</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Is there a polish I can buy that looks like this? Or is Flower Child the closest there is?</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwcpkjtsgpjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1ewfja4</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my best friends nails yesterday </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewfja4</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1ewegzl</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Fave </t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/068apv6o0pjd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1ewe28q</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Blooming gel look with regular polish!!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewe28q</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1ewdni6</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>FINALLY BROKE THE BITING HABIT!!!!!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewdni6</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1ewcad0</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Starrily Neons (Rn, Ne, He, Kr) and  + Plus Life Lacquer's Touch Fuzzy, Get Dizzy</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebrwjupdkojd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1ewbxro</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I now understand the Lorraine hype </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewbxro</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1ewbpb8</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Mooncat Chemical X (3 coats)</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewbpb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1ewblm3</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Baroness X Octo-Alien magnetized two ways!</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7p81w641gojd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1ewb4a1</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe for Ethereal </t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewb4a1/dupe_for_ethereal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1ewb2qq</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe for a discontinued product </t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewb2qq</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1ewayz7</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Seche Vite?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewayz7/seche_vite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1ewashj</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Slug Bug 🩷</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewashj</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1ewadjb</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>KbShimmer polish not drying?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewadjb/kbshimmer_polish_not_drying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1ewa1o8</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Mermaid Nails</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/je6fp4by4ojd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1ewa1ly</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>How do you cope with the “need” to buy more nail polishes?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewa1ly/how_do_you_cope_with_the_need_to_buy_more_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1ew9zyt</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Quarter of a Cent Cherry dupe?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ew9zyt/quarter_of_a_cent_cherry_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1ew8fcd</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>gel removal advice?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ew8fcd/gel_removal_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1ew7ctp</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Lurid’s Burdock and Buckthorn is incredible</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7zrjhqnlnjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1ew72x9</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Poll: if your nails peel/delaminate and are you on birth control? </t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/s/UNFqN8CbpG</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1ew6lmb</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Niagara Falls inspired 🌈</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew6lmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1ew650c</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t xml:space="preserve">does anyone have this nail lamp &amp; would you recommend it? </t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5ov2orzcnjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1ew5my6</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Emerald Amethyst Dreams: Jewel-Toned Nail Magic in Purples and Greens</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew5my6</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1ew5e7s</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>gel polish recommendations?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ew5e7s/gel_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1ew5chv</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Vegas Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew5chv</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1ew59mg</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opi - glazed and amused </t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew59mg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1ew4yvr</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Who’ll stop Lorraine??? 😭</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b19wuzwr4njd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1ew4uar</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know what polish this is? My friend got them done at the salon but doesn’t know the brand/color. She said it’s a very very light blue. </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwtu3btv3njd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1ew4p15</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>You already know this one - 🌸👶</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew4p15</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1ew4i4z</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>when your nails match your favorite shower gel 💚</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew4fxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1ew4d9d</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>🌸🦋✨</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew4d9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1ew47on</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>I was aiming for ethereal and think I "nailed" it</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k538bg5ezmjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1ew445j</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>🌱✨</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew445j</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1ew40xz</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Underwater Grove 🌊🌸</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew40xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1ew3zen</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Best bang for your buck brands?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ew3zen/best_bang_for_your_buck_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1ew3kbp</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for this nail polish </t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8ix3xkbumjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1ew35zl</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Why does this keep happening only on the pinky??</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew35zl</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1ew3166</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Phoenix polish dry time?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ew3166/phoenix_polish_dry_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1ew225e</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Polish recommendation 🗽</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew225e</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1evzyxl</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Is there any nail polish making class? (UK)</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1evzyxl/is_there_any_nail_polish_making_class_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1evzd7s</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Matte spots on swatch dots fixable?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1evzd7s/matte_spots_on_swatch_dots_fixable/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1evza17</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Truth or Dare</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1evza17</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1evxyvs</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1evxyvs/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1evxk66</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Help - what is the difference between 70 and 110 color natural indigo self levelling gel?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1evxk66</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1evx82e</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Zyler Cat Eye on my shorties 🐈</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud1j7s8i7ljd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1evwy58</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Going into the week with donuts 🍩</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1evwy58</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1ewpelg</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Rabbit 🐰</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewpelg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1ewnf6h</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sets </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewnf6h</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1ewlhr2</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Different asthetics</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwlzpmddmqjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1ewlerk</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5wxsi2llqjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1ewkt9m</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Getting ready early for Halloween 🩸🩸🩸</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewkt9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1ewkg4b</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Nail Update</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gn0t1wo3dqjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1ewisty</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Neon Butterflies</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewisty</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1ewgp4w</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pretty proud of how these turned out, still learning! </t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyce6m3uhpjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1ewfryf</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spookey season is coming! </t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvu55a4capjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1ew9na4</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Galaxy toes!</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uq7incq32ojd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1ew9aql</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Bridesmaid set</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew9aql</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1ew9aev</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Painted my nails for the kitties at the shelter I work at</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ew9aev</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1ew85f7</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>What do you think? Too much?</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6egetwkernjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1ew40js</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">M 18 first time doing nail art </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qm9om40ymjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1evyw7t</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>✨🎀⛓️ Pink / Molten Nails ⛓️🎀✨</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r27kynhbrljd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Aug 21 08:09:51 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_25.xlsx
+++ b/data/2024_08_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C476"/>
+  <dimension ref="A1:C637"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8525,6 +8525,2743 @@
         </is>
       </c>
     </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1exjffc</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Ombré on short nails, was a fun experiment, but I guess this would look more flattering on longer nails 😅</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06h3lffpyyjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1exjd49</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving this new color! </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exjd49</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1exj09j</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>2000’s French tip opinions</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c57lrwurtyjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1exir0e</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>I'm obsessed with red ♥️</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4zagjqqqyjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1exigg7</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Do you like kinda clear set??</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxnk0hj9nyjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1exgvt5</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>how can i get nails likes these ? credit @/gracesyn on tiktok :)</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exgvt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1exh2ks</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rainbow French 🌈 </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exh2ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1exges4</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Aprés PSA</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exges4/aprés_psa/</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1exgj8o</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Did press-ons for the second time ever, no tutorials. Be honest,  how did I do?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3rlwgb72yjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1exg944</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>4 years ago, was a chronic nail/cuticle chewer. i’ve officially busted the habit!!!</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exg944</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1exfy1l</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Getting into press on nails, any tips would help</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exfy1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1exfwu1</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>How to take dip powder nails off</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exfwu1/how_to_take_dip_powder_nails_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1exfgid</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>SpongeBob nails (by me, on myself)</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4m4mznpzrxjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1exffnn</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>some of the nails ive made these past few months :D</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exffnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1exejkz</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bubble bath - opi </t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qncjqteyjxjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1exdwwa</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Two from today!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exdwwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1exdm10</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Halloween nails start meow</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wlvi0zm2cxjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1exdhmd</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Finally have healthy nails again!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnz6g2rzaxjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1exd947</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Love this color</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2j3hbk9x8xjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1excxlb</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>My barbed wire nails!!</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1excxlb</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1excmej</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Tried some mushroom nails 🍄☺️</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ryr0fuj3xjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1excgz2</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for the post on nail care </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1excgz2/looking_for_the_post_on_nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1exbtah</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kirby Nails! </t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ok8sxkpwwjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1exbt5f</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Surprise nails I made for my stepmom!</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxdp8z1owwjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1exbdj4</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>fresh outta the jacuzzi. 💜🌸</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yv0wxle0twjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1exb7tg</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silver chrome powder </t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9w7vwk8prwjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1exb103</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>look my new babies, what do we think? 😻🩷</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exb103</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1exb0iu</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Practicing with my nails </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqsky893qwjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1ex9fq3</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Can’t stop this peeling…</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7revibrdwjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1ex8cap</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to not have white tips </t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ex8cap/how_to_not_have_white_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1ex9yku</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Obsessed with orange this summer 🍊</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvhmexcphwjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1ex9la6</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ouija board nails! </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex9la6</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1ex7ild</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starset inspired </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex7ild</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1ex7ix9</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Hey guys!</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex7ix9</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1ex91a7</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>DND #243 Purply Pink</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ex91a7/dnd_243_purply_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1ex8zgz</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>pastel shades</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2k7t3tdawjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1ex8tb0</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>💚</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egbjgsf19wjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1ex8msm</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>What do you think of these claws?🐆</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cyyqjhcr7wjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1ex8kv5</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t xml:space="preserve">uñas de hoy </t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgxnqrmd7wjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1ex8723</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Back to nubs 🥲😭</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex8723</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1ex7sew</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Didn't like the clear ones so went to something simpler</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex7sew</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1ex7p1g</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Bojack horseman set I did 💅</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex7p1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1ex7fct</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Beetle who!?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b721jodwyvjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1ex748b</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alright I take back my hatred of almond </t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3v0x0o4mwvjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1ex6bru</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts pls! </t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex6bru</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1ex65dq</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Newest acrylics</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98mv918rpvjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1ex62xs</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very cutesy very demure </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q82brkeapvjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1ex5fov</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m going to miss this set! Fresh pic +2 week check in </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex5fov</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1ex604y</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>sheer pink gel ex 💗</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex604y</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1ex4m7d</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Classic design but made by me. Do you like them?</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f816f8qsevjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1ex4inj</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink French </t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9x3xwuw2evjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1ex4hk3</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got a purple french tip with lavender polka dots </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9l3fy4xudvjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1ex3twg</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💜 </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxaoyq839vjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1ex35lb</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Pearlescent Pink Nails 🫧💕✨️</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2un6o7a4vjd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1ex2u94</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Might not be everyone’s cup of tea, but I’m really loving this set 🥹</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex2u94</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1ex2m87</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did a friends nails today! </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2e1541se0vjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1ex2arx</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Sorry, just in love with these😭</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bb0vji8yujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1ex24eh</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Is It Too Late?</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex24eh</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1ex1whv</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set of nails </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ph9bsyudvujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1ex0xoq</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>One last bright color before August ends!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmwnsy9joujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1ex0uxa</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Nails I did </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex0uxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1ex0rwj</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>I love this color.</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/800q102hnujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1ex0jj4</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Gel polish mani</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xtjcmmvlujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1ex03uv</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Found the best nail glue for press on nails. Usually with other glues my nails will fall off within a couple days. I have had these for almost 2 weeks and none of them have come off or come loose. It's called Curve Life. It's semi-solid and also comes with remover.</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex03uv</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1ex05rk</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Thoughts? 💚😍⚡️</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqe5ui3ajujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1ex035v</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>1st 2nd or 3rd</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykg4a4esiujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1ewp0w8</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SOS I need help damaged nails </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewp0w8/sos_i_need_help_damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1ewq82e</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Villainess inspired nails ✨ </t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewq82e</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1ewztva</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>So cute and so cheap!</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv4dp8ntgujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1ewzhpw</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">💅🤍 </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewzhpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1ewz8a4</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Fall nails</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04xrvrjscujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1ewz7pi</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Thouths? 💚😍👾</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/213m5c8ocujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1ewz0kk</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Bday mani!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewz0kk</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1ewyzq2</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>5 day old Glamnetic press ons</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abbez9f1bujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1eww9ud</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Why does my rubber base turn yellow after a while?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eww9ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1ewway0</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Crackle nail polish</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/92cmdylvrtjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1ewyzka</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Summer’s Last Hurrah</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewyzka</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1ewyg2u</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>I'm calling it a punk French mani</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewyg2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1ewydkz</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Cherry coquette nails🍒🎀</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewydkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1ewxuk6</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Did cateye nails on my natural nails for the 1st time.</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewxuk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1ewxrhe</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Summer is fun but I’m looking forward to *demure* Fall shades.</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewxrhe</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1ewxmsw</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Please critique - DIY #15</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewxmsw</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1eww9qc</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Cat eye french tip!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eww9qc</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1ewvxq5</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>delicate nails</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1xp90fb3ptjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1ewvry2</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">new manicure :) i’m just really happy with how they came out, ive been going to a new nail salon and every set ive gotten from them ive loved! (this is a DND polish i believe the color is pearly pink but i don’t remember 😔) </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewvry2</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1ewvcn0</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silver gel nails </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewvcn0</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1ewv0gv</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>First time using fiber.</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynzkf9t4itjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1ewtcrx</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>I think this set is going to rock the club</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewtcrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1ewt86y</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>pricing advice</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewt86y</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1ewt1hz</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Blue simple french with a twist. What do you think? 💙</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lvzpusi0tjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1ews9lc</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail breakage </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ffxxxno6ssjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1ewrx81</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>First time trying BIAB</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9t22e58osjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1ewro48</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Tried press on for the first time</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewro48</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1ewqmgr</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Summer vibes～</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewqmgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1ewq9mh</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Acrylic on natural nails - how many infills can I get before a soak off and new set?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ewq9mh/acrylic_on_natural_nails_how_many_infills_can_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1exis0k</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Are gel extensions better than gel on natural nails?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exis0k/are_gel_extensions_better_than_gel_on_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1exia3v</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ripe dragon fruit color? </t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exia3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1exi1ty</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Katerina Beauty number 020</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/k-b-number-020-3ut6ta1</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1exhz4s</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Katerina Beauty number 010</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/S8I79yr</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1exhbb2</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s your fav brand you’ve discovered through PPU? </t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exhbb2/whats_your_fav_brand_youve_discovered_through_ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1exh01e</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Demure rainbow 🌈 </t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8kmdzde17yjd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1exgomx</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>It’s not just me right??</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p15hhknq3yjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1exes1v</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Looking for a dark red jelly</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exes1v/looking_for_a_dark_red_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1exdkxq</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Swatched my collection!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exdkxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1excyh2</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nails for school </t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1excyh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1excso7</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Lūmen Glass Frog</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1excso7</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1exc9ya</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Buckle Up, It's Round-up Time.</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exc9ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1exc44a</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>the famous combo...</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exc44a</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1exbovh</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Freshly Bitten is so good 🫦</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exbovh</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1exbcu5</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Magical girl transformation polish </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exbcu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1exbcu3</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>fresh outta the jacuzzi. 💜🌸</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb6l5zwuswjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1ex9w1k</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Guayaba jelly 💖</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjpwj6z5hwjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1ex9gmi</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Love the color, hate the formula - best deep reds?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04mpccxydwjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1ewtixh</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>I saw this color on a thread about favorite job interview polishes. What do you think? Would I get the job?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5ats1a95tjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1ewvqft</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sally Hansen Miracle Gel SHHHH-IMMER dupes? </t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1g42kglntjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1ex1ol1</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chipping help! </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/026zgl6ttujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1ex86ks</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Layering is fun! </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnqijjji4wjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1ex7gtz</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>What nail shape for nails that bend down?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex7gtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1ex7gsn</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s the best opaque white polish for nails? </t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ex7gsn/whats_the_best_opaque_white_polish_for_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1ex7gig</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>babys first lynb order</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex7gig</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1ex6i5y</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse (H) vs. Mooncat Gates Of Hell</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ex6i5y/ilnp_eclipse_h_vs_mooncat_gates_of_hell/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1ex6ggo</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Thoughts on this situation?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95tvvn6xrvjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1ex62l4</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>My first ILNP!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am8lfpp6pvjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1ex5w15</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ex5w15/death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1ex5uef</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>What’s the difference between base coat and top coat?</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ex5uef/whats_the_difference_between_base_coat_and_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1ex5fw4</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Pop arazzi sticky adhesion base coat - is it Polyvinyl Butyral free?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ex5fw4/pop_arazzi_sticky_adhesion_base_coat_is_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1ex5cs0</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Best indie dip powder brands?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okdgxz84kvjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1ex49sn</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>plain pink jelly dupe for blossom's firebreath from mooncat?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex49sn</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1ex3wwa</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Jello</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex3wwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1ex29j4</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Would you ask for a refund ...?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ex29j4/would_you_ask_for_a_refund/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1ex1ae0</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Switched to a Russian salon </t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9txig6l1rujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1ex0wx2</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Sally Hansen Insta Dry Go Garnet but jelly?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ct9q17i9oujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1ex066k</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Gunmetal on shorties</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u0kbzi2djujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1ex03ml</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should have bought a horseshoe magnet earlier! </t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ixvk17yuiujd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1ewznnb</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Patchy or another coat? </t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssh98f6rfujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1ewz0nm</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Have we talked about ILNP Abracadabra lately?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4m99acg5bujd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1ewyrxl</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Brat Roses</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewyrxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1ewynn5</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>🧡💛Aldi Stripes🩵💙</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewynn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1ewyhjp</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Please help me to describe this color so I can find a dupe (Pacifica Fierce Femme)? Info in comment</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/I/61pcsOIiJnL._SX679_.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1ewygsl</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Peridot for the August babies</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewygsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1ewyehf</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Power Surge ⚡️ </t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewyehf</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1ewwm5n</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My ombre is so subtle the camera barely picks it up </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewwm5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1ewwhn6</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Savoring shifty goodness to combat the chaos that is flying through DFW</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcps9is8ttjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1ewvotu</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Mini?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ewvotu/dazzle_dry_mini/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1ewvctq</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Cappuccino Clouds</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzzkf5qlktjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1ewv78z</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>The most high-stakes nail painting I’ve ever done</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewv78z</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1ewv5ac</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opi Top Coat not dry after 4 hours, switch to QDTC? </t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idr61ao6jtjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1ewutuj</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple-gray skittle </t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewutuj</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1ewuh7b</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>My favorite polishes of all time</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewuh7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1ewt9cc</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Nail art ideas? These feel ... unfinished.</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o80sc74o2tjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1exga6w</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Anyone have any idea what these are supposed to be?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dvldwjpzxjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1exfd9y</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>SpongeBob by me (on myself) - pro nail tech</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9yudjr6rxjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1exf0xs</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Blue princess nails</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exf0xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1exax5u</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Lime Nails</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exax5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1ex9m18</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ouija board nails! </t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex9m18</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1ex54l8</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beginner fall nails </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ex54l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1ex0jgl</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Finished Nail Set!</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/01kx8e7vlujd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1ex06kn</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>September Nails?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ex06kn/september_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1ewywef</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Need help figuring out which practice hand to get</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewywef</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1ewrq35</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do yall think? </t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewrq35</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1ewqn93</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Summer vibes press on</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ewqn93</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Aug 22 08:09:25 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_25.xlsx
+++ b/data/2024_08_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C637"/>
+  <dimension ref="A1:C803"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11262,6 +11262,2828 @@
         </is>
       </c>
     </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1eyds63</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>In love with stiletto shape nails</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/los279aea6kd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1eyay64</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Nail extensions without nail glue</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cz9an1gc5kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1eybo7t</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>trippy freestyle! thoughts on matte top coats ?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eybo7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1eybhcl</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Hard Gel - Chrome and Cats eye</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bcxo6nai5kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1eyb2jw</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>My new set turned out so cute! I think I did a better job on the flowers this time too and even went a little extra with the bead in the centers 🥰</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvy2okeqd5kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1eyay5h</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where to find  Snoopy/Peanuts Charms </t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyay5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1eyasr7</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Nail Shape Recommendations</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyasr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1eyaqsq</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do almond nails suit my long skinny fingers? </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lelj0b9ba5kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1eyajvd</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Pink cateye /velvet nails 🩷</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y7c817wd85kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1eyagki</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>My nails keep breaking dangerously short for no reason</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyagki</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1ey9wuo</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>New set of nails</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okt48r3925kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1ey9ggq</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>spooky zombie nails anyone?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gisv0umrx4kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1ey8f6v</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Looking for bird claw nails near DC!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ey8f6v/looking_for_bird_claw_nails_near_dc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1ey8drv</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Been searching high and low for this shade of pink in OPI specifically!! 🙏</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bz3jxxr0o4kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1ey7zdj</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>I’ve made the casting on the nail the first time😍</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mli4q95hk4kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1ey80wj</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Is this how acrylic nails are supposed to be angled? They look strange to me.</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sveg3guk4kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1ey7v3j</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>best jelly/gel like nail polishes?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ey7v3j/best_jellygel_like_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1ey6zsk</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Sparkly Purple 💜💜</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gh3ykyy3c4kd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1ey6zar</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Red color block</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v12zgd20c4kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1ey6wvd</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>I do myself. 😊</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/likz2u4fb4kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1ey6vd7</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>My new nails! Does it look like press ons?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey6vd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1ey6bi8</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Super delicate. How much from 1 to 10?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onb5oc4i64kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1ey68l1</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>All matching, but they look so fake</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vid3q5fs54kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1ey68cf</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I really liked my new nail design, super simple </t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9l1tjldq54kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1ey5wmt</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me better?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey5wmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1ey5wi2</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reasons why chrome comes off? </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u3w93by24kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1ey5w9k</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Gel x normal?</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey5w9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1ey5kjb</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glitter girly nails </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzx2xui504kd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1ey5jk4</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Jade marble nails✨</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mudgk0axz3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1ey4z53</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Got a manicure for the first time and…</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ey4z53/got_a_manicure_for_the_first_time_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1ey560m</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eyes.  Magnets are hard! </t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ontmk1msw3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1ey4wwb</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manicure for summer ☀️ </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oktku46qu3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1ey4btc</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Needed a change! New/old nails</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey4btc</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1ey4563</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Asked for a sparkly nude for this fill and she did not disappoint 😮‍💨 by @ nailsbyxoyanie</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/updtkpgeo3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1ey40xa</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Red Nails is Beautiful and…</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wfhz7lgn3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1ey3evw</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to be more bold in my color choices. Thoughts? </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtfof85si3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1ey2dti</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>There is no greater pampering than getting your nails done, I think it improves any outfit 100%... by the way, a fan of the stars, can you tell?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey2dti</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1ey2bcs</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>On Wednesdays we wear pink</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kp9by4ja3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1ey25n4</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic nails popping off </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ey25n4/acrylic_nails_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1ey1qg6</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First dip powder set </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3dt8gc563kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1ey20hi</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Had some leftover shiny plastic</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t2rzxbk883kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1ey1z2g</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>first full freestyle/original design as a tech!</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey1z2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1exzsfv</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Frog acrylic set</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exzsfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1ey0o9f</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>BIAB not lasting on my nails</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ey0o9f/biab_not_lasting_on_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1exzygs</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If you were a client going to at home based salon would you be okay with this? </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exzygs/if_you_were_a_client_going_to_at_home_based_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1exwylu</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail growth question </t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exwylu</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1exxtqb</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">simple but beautiful design </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/toy9216xd2kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1exxhhz</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>How’d I do?</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exxhhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1exxga0</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opening Nail Salon - Looking for Gel/Polish/Dip Recommendations </t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exxga0/opening_nail_salon_looking_for_gelpolishdip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1exxamj</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Third time making press ons, I decided to theme them after a book this time ☺️</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exxamj</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1exx5im</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Quick question!</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exx5im/quick_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1exx13p</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Color leopard - pedi sets serie #2</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phkydgo782kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1exwrfo</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>any advice?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4gacla962kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1exu00i</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Nail dip</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exu00i</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1exwj9b</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don’t know if I like them or not, they remind me of these cookies. </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exwj9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1exwgmg</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>More pix of the cutesy almonds</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exwgmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1exwgd4</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stupid question for you </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exwgd4/stupid_question_for_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1exvr1r</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Warm n' Cold DIY overlay </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exvr1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1exv16c</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>When you live for being extra 💅</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14zmvo51u1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1exufcy</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I did these myself. Are the stickers too much? </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exufcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1exuf3a</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>I regret these colors 😳</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buvjqdgrp1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1exudwd</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautiful and simple set I did for my bestie </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynsw1nejp1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1exub5j</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Medium denim blue available in the US ?</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exub5j/medium_denim_blue_available_in_the_us/</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1extunt</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>DIY nails/beginner</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/548t1hpol1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1extpai</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was going for some abstract but clean line designs. I like what my tech came up with! </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1extpai</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1ext403</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Some of my favorite designs this year!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ext403</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1exsqjx</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Gel Nails Lifting (Salon)</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exsqjx/gel_nails_lifting_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1exsl5u</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Turquoise nails 💅 </t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v18l0cxxc1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1exshj9</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Violet nails</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7uzvjc7c1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1exsd2t</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green marble 💚 </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exsd2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1exryxo</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel nails while pregnant? </t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exryxo/gel_nails_while_pregnant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1exrt4x</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Anyone else notice the change in Una Gella nails sold on Amazon?</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exrt4x/anyone_else_notice_the_change_in_una_gella_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1exrbz7</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>i can’t stop staring at the sparkles</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eo2jtm441kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1exr5pa</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>new and my favorites🖤</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/np5wjjuu21kd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1exp4r0</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>how to file "nail bed"</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exp4r0/how_to_file_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1exr1pu</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Ocean water nails 🌊✨</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exr1pu</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1exqyyh</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Process of painting Emily 💙🕸️</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exqyyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1exqsya</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Simple dots. 🩷</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exqsya</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1exqodl</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Alcohol percent to remove tacky gel top layer??</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1exqodl/alcohol_percent_to_remove_tacky_gel_top_layer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1exqihq</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What's causing this fine wrinkling? </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exqihq</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1exq4r7</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>back with another set</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exq4r7</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1exq4qg</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black &amp; Gold Chrome </t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49ii5f02v0kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1exph4h</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Classic</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exph4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1expgau</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Kokoist users</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1expgau/kokoist_users/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1exoyv7</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Another little try out</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8r0vkzyl0kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1exo27o</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Best Nail Art Artist </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjxn8bnae0kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1exn2pq</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Critiques? </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exn2pq</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1exm6ce</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Blue swirls💙</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfi5dwisvzjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1exl30b</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>RIP to my natural nail growth😭</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo2fvyxyizjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1exk5wt</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Finally long again</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exk5wt</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1eycphi</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>After months of futile attempts to fight my gel allergy and several bad reactions, I gave up and am now back to regular polish. I finally found a polish that reminds me of my favourite gel mani, "Gilded Galaxy" by Essie. It cheers me up a little.</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5xuraixw5kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1ey6eyq</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Curious about Reusable Press-Ons</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ey6eyq/curious_about_reusable_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1exwsx2</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Holo Taco Mint Mojito</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exwsx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1ey97uf</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m loving this color! </t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey97uf</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1ey8yu0</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Feeling the fall vibes already 🍂</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey8yu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1ey83i9</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Birthday shorties after salon damage</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey83i9</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1ey7xv0</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lumen Varis </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey7xv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1ey6ozj</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Not sure why I didn’t try this on sooner!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey6ozj</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1ey5wln</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>thumbs splitting down middle of base</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ey5wln/thumbs_splitting_down_middle_of_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1ey4joo</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>After nearly giving up on stamping</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/WmrjYhI.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1ey4jl0</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Game over </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i64w06unr3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1ey3jzl</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Best nail polish base?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ey3jzl/best_nail_polish_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1ey2cf4</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Touch of pale pink</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6os6fz1qa3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1ey1wea</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Glasswing Butterfly 🦋</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gexz38ge73kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1ey1ixd</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Coraline claws 💅🪡</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnn8649n43kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1ey0iqx</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>The Sky is Falling</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey0iqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1ey0bgy</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Deep Space Magic 🌟☄️</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/17xhf4gsv2kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1ey08gb</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DND #243 Purply Pink </t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ey08gb/dnd_243_purply_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1exzyg1</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque response </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exzyg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1exzx37</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Is there a difference between top and base coat?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exzx37/is_there_a_difference_between_top_and_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1exzhe1</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Starterset Pink Gellac - Worth it?</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxzdopfqp2kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1exydo4</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>alright, what’s the best nail oil?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exydo4/alright_whats_the_best_nail_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1exxymy</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cherry cola </t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exxymy</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1exxsyk</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy sauce - Chicago fire </t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exxsyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1exxrnj</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Finally found the sparkly neon green combo I’ve been searching for!</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exxrnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1exxqf5</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Matte flowers 🌸 </t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exxqf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1exxipy</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DVN But Do Aliens Believe In Me? </t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exxipy</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1exxi04</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>We have Flower Child at home</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exxi04</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1exwif9</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌊🌌 I missed playing with fluid art!! </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exwif9</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1exve7t</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Surprised by how much I love this one </t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fay4q7pkw1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1exuwj5</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Teal greens with pink flakies</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exuwj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1exutht</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Help! I have really brittle natural nails and my cuticles are a mess</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvau36els1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1exuffi</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Don't sleep on the dollar store, ladies and gents.</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exuffi</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1exu3n6</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Which first: ridge filler or rubberized base?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exu3n6/which_first_ridge_filler_or_rubberized_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1extegx</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Matte Sin Eater</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdc21cani1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1exte41</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Rainbow Connection Reviews</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exte41/rainbow_connection_reviews/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1exswbd</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Emily De Molly "Silent Breath"</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87orucvwe1kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1exs21a</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>I'm not loving...</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exs21a</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1exrn82</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>This is supposed to be pink</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exrn82</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1exrk1p</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Help with discord</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exrk1p/help_with_discord/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1exreqd</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Swatched and Organized. Can you tell what my favorite color is?</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exreqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1exrcl9</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>strawberry girls 🍓</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exrcl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1exr90r</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Found my perfect red ♥️</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6ub7k3j31kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1exr2km</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>First indie polishes!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exr2km</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1exr17k</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">finally caved and acquired a horseshoe magnet </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u65nmtqs11kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1exqo1n</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Cirque Colors reposted @lacquerdiary3.14’s comparison swatches of the new Jarritos collection but edited a photo to make it look like there’s more of a difference between two shades</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exqo1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1expx9c</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clinique black honey nail Polish suggestions </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik9of6xet0kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1expt88</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>🔥Fire Tips🔥</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1expt88</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1expqdf</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Fuchsialicious 💖</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1expqdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1exost5</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethereal forces - Emily de Molly </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cj5gxq6jk0kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1exopt3</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj2n7njuj0kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1exoiiz</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Sparkly Watermelon</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exoiiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1exn13r</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Why is my polish chipping after one day?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exn13r/why_is_my_polish_chipping_after_one_day/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1exlns6</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Please help, how could I create this effect??</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4ou4b81qzjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1exd9yo</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Low maintenance nail ideas?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1exd9yo/low_maintenance_nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1eycw2q</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Black n blue</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5gm60o6z5kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1eybv20</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Miffy nails!</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbvyw1oom5kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1eybntp</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>First time trying magnetic polish 💅</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eybntp</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1ey93zk</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>NAILS</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey93zk</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1ey7t8u</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Jade marble tips</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey7t8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1ey6nbg</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Art </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/btqqkhc794kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1ey5zpy</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Full simple nail art🖤✨️🥵 what do u think?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8q4b2mp34kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1ey54fg</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried some funky nail art today. </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xboguy2gw3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1ey2zfv</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Three Coats, and I’ve found my holy grail pink! (DND884)</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9h6k91jf3kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1ey1w6g</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beachy 🌊 </t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey1w6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1ey1jau</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Coraline claws 💅🪡</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/et5t360q43kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1ey0skh</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Fun stuff this week ✨</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ey0skh</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1ey074i</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>DND #243 Purply Pink</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ey074i/dnd_243_purply_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1exzkg7</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>I did the Aura Nails!</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5be2sjhdq2kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1exx1p9</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Color leopard - pedi sets serie #2</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ku8re1c82kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1exwj5v</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Random nail set </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1exwj5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1extqzq</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haven't been this happy birthday with a set in awhile </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1extqzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1exs3x0</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Finally found a top coat that doesn’t wash out my fancy foils</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/embkx6sl91kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1exp23e</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>What type of nail art is this?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ow1wjgnm0kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1exmg18</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Who doesn't love pink 🌸🩷</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bj8lpzvnyzjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1exlmx4</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How would I create this effect </t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bh90a6qpzjd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Aug 23 08:10:16 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_25.xlsx
+++ b/data/2024_08_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C803"/>
+  <dimension ref="A1:C957"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14084,6 +14084,2624 @@
         </is>
       </c>
     </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1ez6cty</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Surprisingly pretty 3$ holo glitter</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez6cty</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1ez5qie</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Attempt no. 6</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez5qie</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1ez59vz</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Nails lifting within days</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez59vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1ez50v9</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Eleganté</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez50v9</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1ez3o1d</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Feeling like skittles</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2660zabackd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1ez4mr7</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What should you expect during a nail appointment </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ez4mr7/what_should_you_expect_during_a_nail_appointment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1ez30o5</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Rate my nail experience. Bitten. Acrylic. Solar powder. Shellac. Info in Comments.</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez30o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1ez2qm7</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t xml:space="preserve">short milky white🥛 </t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zj7ya7kd1ckd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1ez2p2q</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail care routine? </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ez2p2q/nail_care_routine/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1ez228e</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dried flowers with French tip pink gel for my wedding. </t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dab8n26vbkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1ez1tio</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>For all the teachers…</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/782zxuj1tbkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1ez1app</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>sunflower szn 💛</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez1app</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1ez1900</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>New set 🌀🌿🍇🏵️</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez1900</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1ez137z</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Looking for Design Ideas</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez137z</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1ez0ysf</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My most recent nails </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfd92x6flbkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1ez0lud</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>feeling really bratty before the summer ends 💚</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez0lud</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1ez0apt</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>First set in 6 months🥹</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o834l8qnfbkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1eyzxah</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Clásic🥰🥰</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqelkktdcbkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1eyyfkp</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Always smearing?</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyyfkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1eyzmuw</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>my last two sets have been some of my faves ever 🙈💕</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyzmuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1eyytaq</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Berry color for end of summer</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyfqyo923bkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1eyyqbn</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Gel nails for the first time in 19384930 years</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrxzldld2bkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1eyyfxa</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Coraline Nails 🥲✨</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yi8l2qvzzakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1eyyazx</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Joker nails.</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyyazx</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1eyxvoq</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>lol cute nails scary pose</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyxvoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1eyxrmy</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love how shiny my nails look with this polish </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tpyrb8juakd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1eyxqhc</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">green chrome and star charm nails ~ </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dyu6qqcauakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1eyxarr</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out square nails for a change </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88i7ogdsqakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1eyx98y</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Emerald color, what do you think?</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpepgcvgqakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1eyx7kq</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Cute cats and glitter 🥰 by me</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vorduce5qakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1eyx57t</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>my new nails</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyx57t</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1eyx2q5</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t go wrong with this color </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyx2q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1eywg28</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Just Got My Nails Done , They’re So Cute!</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/przi05d3kakd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1eyw58t</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>weird pealing on natural nails</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyw58t</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1eyw3vq</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>New new</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzo9w84khakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1eyvvw4</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Gothesque</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyvvw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1eyvgge</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Ohh, it was very difficult 🖤⛓️</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyvgge</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1eyvfp5</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Hand painted neon paisley!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyvfp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1eyvfm3</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Galaxy nails 🪐🩵</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlc2j9adcakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1eyvdqp</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>how to know which kind of nails i got??</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iq84hfhybakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1eyv3tp</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Cute or flop?</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyv3tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1eyv1n5</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Why does it feel like all my nail techs get sloppy after a year?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eyv1n5/why_does_it_feel_like_all_my_nail_techs_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1eyuz9w</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>My first soft gels to my mom!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyuz9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1eyu5xl</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Got biab done for the first time - should it look like this?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyu5xl</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1eytvfj</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">feeling so discouraged. how are you guys neatly and nicely applying press on nails with glue? i feel like i can’t win. </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqv9mw7k0akd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1eytdn0</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i love jelly + glitter lately ✨️ </t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nis1zrxxw9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1eyt1rm</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had to take photos before I destroyed them at work </t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyt1rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1eyt0us</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Nail shape ok for guy hands?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mml71rgdu9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1eys5m3</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>First time trying almond shape 😊</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eys5m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1eys206</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time at age 24, now I understand the obsession - I can’t stop staring at my nails and I’m so happy :)</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p59vwqe5n9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1eys1kr</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went out of my comfort zone and only 50/100 regret </t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eys1kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1eyrrr0</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Sailor Moon nails!</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyrrr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1eyrfhw</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Started to do Matte Finish</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkdkn2wki9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1eyrbib</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do u guess think ? </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id19jdnrh9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1eyr85k</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been soo obsessed with 3D gel lately </t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ia8qlvc2h9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1eyr59d</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gave my SIL creative freedom. </t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nu3gffzgg9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1eyr4dg</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Simple, but I love it!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyr4dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1eyfa72</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t know how to ask for what I want in the salon. </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eyfa72/i_dont_know_how_to_ask_for_what_i_want_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1eyl90t</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Can someone recommend an acrylic kit?</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eyl90t/can_someone_recommend_an_acrylic_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1eyqefy</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>This set really grew on me ✨</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyqefy</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1eyp7y5</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>🫠🤎 (+inspiration pic)</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyp7y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1eyq6mz</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Press Ons for Smaller Nail Beds</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzyggdsg99kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1eypjfm</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>I let my daughter choose the colour of my nails.</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eypjfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1eyou4i</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Nail prep advice</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cnu3el5sz8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1eyp4bg</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>nails based on the sistine chapel</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib73zp0s19kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1eyp3qo</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>🪸🐠🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kp57y3gp19kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1eyobpq</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Tangerine 🍊</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1m1g251bw8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1eynsyx</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>How does russain nail manicure make your natural nails more “healthy”?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eynsyx/how_does_russain_nail_manicure_make_your_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1eynsqy</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Cunty Nails🩷</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvcpspcns8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1eyno98</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>First time doing my own nails!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ll3p0x3rr8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1eynefi</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Second time ever doing gel nails - took advice from people here and used a base + top coat. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2pvalhtp8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1eyn8he</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>My tech gave me koi fish nails for my trip to Japan</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e01bzpnoo8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1eyn6s1</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpnu88gco8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1eymzbd</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Tried the velvet nails 🧲 trick.</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a8ysz6hvm8kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1eym668</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Does anyone know who sells nails as small as the XXS size small of Olive &amp; June press on?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hc0dc0x2h8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1eymfw0</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>did these myself, natural nails!!</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eymfw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1eylm6r</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Do you like this print?😍</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5xi5am3bd8kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1eykr2q</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My friend did my nails yesterday so pretty:) </t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6qe52n278kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1eykox0</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>so the last week i’ve been trying nail art for the first time!</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eykox0</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1eyjcjg</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neon French Gel </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyjcjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1eyibpe</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry Picnic 🍒 🧺 </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyibpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1eyhm7m</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Nail rookie and recovering nail picker, do I choose gel or dip powder?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eyhm7m/nail_rookie_and_recovering_nail_picker_do_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1eygumg</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Trying to rescue my nails. Looking for growth serum or clear coat recommendations</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eygumg/trying_to_rescue_my_nails_looking_for_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1eyencf</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>corseted set w/ a kawaii touch !!</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/55cdmi6cl6kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1ez6jzr</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Klein Blue</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ji029g1a7dkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1ez69j2</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shall I contact these online shops to correct their description about hema content? </t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ez69j2/shall_i_contact_these_online_shops_to_correct/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1ez5jde</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Moon Stone</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez5jde</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1ez48ek</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Subtle but still fun polishes?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ez48ek/subtle_but_still_fun_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1ez3q0u</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: tortie on natural nails </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez3q0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1ez3g5s</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with the way direct light changes ‘little star’ by bees knees </t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez3g5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1ez3338</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips for cleaning out/emptying bottles? </t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ez3338/tips_for_cleaning_outemptying_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1ez2zqg</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Share Your Manis in Nature!</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dq09dxs3ckd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1ez2gyi</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>ILNP Nocturnal vs. Mooncat Midnight Rider</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ez2gyi/ilnp_nocturnal_vs_mooncat_midnight_rider/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1ez1716</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Red ♥️👹</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez1716</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1ez0z3e</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer GWP</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez0z3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1ez0mwq</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some late summer polishes </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez0mwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1ez0kwv</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Do you use a basecoat?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ez0kwv/do_you_use_a_basecoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1ez095a</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>A Hoot And A Half 💜</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez095a</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1eyzrr1</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Treated myself to a salon manicure this morning. Probably the cleanest manicure I’ve ever received. I love techs who really care.</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8aex73j4bbkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1eyzowf</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer arrived! (Last two pics are mystery bag)</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyzowf</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1eyygkt</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Fire &amp; Ice</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyygkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1eyygdw</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>o7s or Fs</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyygdw</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1eyxynt</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>ILNP Willow deserves more attention!!</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyxynt</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1eyxxx4</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>fairy dust as a topper! (my car is parked)</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/173zcckxvakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1eyxui6</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Help me find a dupe!</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smfmyki6vakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1eyxk16</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Life as a Shrimp 🦐 </t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fr3a232usakd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1eyx5j4</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Colort theory help</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ip5qj91ppakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1eywhs9</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Nails separating because of base coat with PVB</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eywhs9/nails_separating_because_of_base_coat_with_pvb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1eywf6y</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Received a surprise Prototype in my Lurid order! </t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eywf6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1eyvy7m</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>The perfect Fluro pink (and just happens to be my cheapest polish!)</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1r98v4q7gakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1eyvstz</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Manicures &amp; Kickboxing</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyvstz</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1eyuojy</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Galaxies at my fingertips </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/axe8qenn6akd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1eyugg6</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>What Addiction? - Lilac Lullaby Petals</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyugg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1eyu9vp</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Dupe Help</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyu9vp</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1eyu3d2</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>That Emerald Shimmer</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhhnl1q72akd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1eytcmw</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fantasy Fire stash </t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mp0piajqw9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1eysbhd</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>A visualisation of quality control (or lack thereof)</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eysbhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1eyrrpp</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me find a dupe pls! </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47ol6kd1l9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1eyroyx</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>ILNP- MISBEHAVING</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rg4na1zgk9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1eypzz0</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>GERmanikure and mont bleu alternatives in Europe</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eypzz0/germanikure_and_mont_bleu_alternatives_in_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1eypj08</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Y’all nailed it on the dupe request!</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eypj08</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1eype1p</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried the velvet 🧲 trick </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g4f1doqq39kd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1eypcmr</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Tips for painting/beautifying gnarly tiny toenails?</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eypcmr/tips_for_paintingbeautifying_gnarly_tiny_toenails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1eyoz8o</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>I literally gasped walking out in the sun!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyoz8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1eyosh3</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">More Love for Essie Gilded Galaxy with my henna </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyosh3</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1eyopbc</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Where could I find this shade of green?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ieaywv6uy8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1eyoeq3</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Just a plain pearlie palette cleanser</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxv6y2evw8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1eynmf3</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Best Nude for cool fair skin</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eynmf3/best_nude_for_cool_fair_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1eynl6u</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Looking for a color similar to OPI Pisces the Future</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eynl6u/looking_for_a_color_similar_to_opi_pisces_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1eyn671</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>thermal fun :D</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f12t1ey7o8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1eymkqa</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Summertime is watermelon time!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvklt961k8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1eymc42</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Cuticula - Link In Park</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eymc42</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1eyliph</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Your holy grail hand cream? (Winter AM + PM and Summer AM + PM)</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eyliph/your_holy_grail_hand_cream_winter_am_pm_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1eyjipa</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Accidentally matched with my Starbucks cup!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyjipa</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1eyh84n</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried stamping. Am addicted. </t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ccob6wzd7kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1eyftv7</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Can I use ridge filler to smooth over glitter polish?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1eyftv7/can_i_use_ridge_filler_to_smooth_over_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1eye7yu</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lestat at the beach </t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eye7yu</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1eydw52</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Re: Cirque Colors editing swatch photos and colour accuracy.</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eydw52</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1ez733h</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>My first cat eye, happy with the result, would you do it yourself?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48uzbayrddkd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1ez64sj</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>based on coraline</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez64sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1ez3p1h</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY: 2nd time trying tortie </t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez3p1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1ez1d7g</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Marbling ink recommendations </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ez1d7g/marbling_ink_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1ez11s6</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>pigments 🔥</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ie6j6afambkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1ez0wnn</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My most recent one so they both are orange n yellow but lighter shades of each other </t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1izyy3zpkbkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1ez0lch</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>I really love blue nail art, and I'm very satisfied with this manicure. Huge thanks to my nail artist, Meggie, for spending 3 hours creating this design for me! She truly put in a lot of effort with the color blending and gradient work!</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fh6ltwuqhbkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1eyvibd</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>does this look like stones? I tried 🫠</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyvibd</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1eyvhdk</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Hand painted neon paisley!</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eyvhdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1eytip6</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been teaching myself nail art for the last year. A set from earlier on. What do you guys think? </t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqrz3fjzx9kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1eypxlw</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>anyone know a good water color pencil brand for doodle nails??</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1eypxlw/anyone_know_a_good_water_color_pencil_brand_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1eyp2hg</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>nails based off the sistine chapel</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdutr3ze19kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1eyn97x</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zelda themed nail set done by me </t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nbbydmuo8kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1eyl5ve</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Nail stand adhesion</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1eyl5ve/nail_stand_adhesion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1eygun4</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My third ever attempt </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv269ci9a7kd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1eygq5u</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Morgan taylor </t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eygq5u</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Aug 24 08:08:13 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_25.xlsx
+++ b/data/2024_08_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C957"/>
+  <dimension ref="A1:C1128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16702,6 +16702,2915 @@
         </is>
       </c>
     </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ezznt0</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Just find the things that inspire you and take a photo with it 🤣</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etmygansdkkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ezzmoo</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Natural milky nails. I wasn’t expecting to like those as much as I did.</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbuefglddkkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ezzgie</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic clean looking nails ! </t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezzgie/basic_clean_looking_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1ezz6tp</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>❤️❤️</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezz6tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ezylxx</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>What nail shape should I do?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezylxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ezyh8e</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Question about services</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezyh8e/question_about_services/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ezy23h</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Help!! Why isn’t Kerasal working?</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezy23h/help_why_isnt_kerasal_working/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ezxu0j</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Anyone know where to find this shade?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezxu0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ezxfqx</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>My claws survived camping!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qb1k2x7fnjkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ezx9g6</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Manicurist made my nails so square and unnatural!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/i1s8juwfljkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ezx1g2</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Glue-ons for someone who spends lots of time with their hands wet?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezx1g2/glueons_for_someone_who_spends_lots_of_time_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ezwhug</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t xml:space="preserve">AZ Diamondbacks </t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezwhug</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ezwgl6</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Done with summer, give me fall vibes </t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48pmepy0djkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ezwfuc</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>These are my nails. What color should I paint them?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezwfuc</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ezw7km</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t xml:space="preserve">short nail era with french tip </t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfzoc4bjajkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ezw6mw</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting ready for some football! </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0k8nzu9ajkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ezw3je</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>I’m a sucker for Cat Eye polish</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezw3je</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1ezw047</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>my nails for end of August✨</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjtnynvg8jkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1ezvtd0</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">boyfriend let me do his nails! </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dxybvll6jkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1ezvfqq</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">We love pink, do you like it combined with zebra? </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlxgi21x2jkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1ezug00</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Is this gel manicure even good?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3hmrjwetikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1eztf0r</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Belated birthday nails</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eztf0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1ezt0cd</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Aurora Almond Frenchies</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m2lfc2vcgikd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1ezsw79</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Is the red &amp; gold a good look?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tfn35urbfikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1ezsot8</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> {PR} Sassy Sauce | Polish Pick Up - Simply Shreeeik</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezsot8</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1ezs56b</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Advice needed!</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/woys9qpt8ikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1ezs7gh</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>I’m so confused</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezs7gh/im_so_confused/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1ezsdrs</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏾💜</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezsdrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1ezs5en</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>I never knew how unsanitary!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q84vfw2v8ikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1ezs52b</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you think? </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezs52b</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1ezs2f6</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m having buyers remorse. Please hype me up be real </t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z67pb4078ikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1ezrwkp</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Today I got this manicure, what do you think?</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98o0vrp25ikd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1ezrn62</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>First time with long nails. Advice?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezrn62/first_time_with_long_nails_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1ezrl4l</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Virgo Season</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmztpt374ikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1ezouvx</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Question about Beetles Nail Polish for a Hobby/Beginner Tech???</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezouvx/question_about_beetles_nail_polish_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1ezq1dj</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone tried the Rejuvenation Nail Oil from brothers?  </t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezq1dj/has_anyone_tried_the_rejuvenation_nail_oil_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1ezpswh</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>What do I do about these :(</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kqa0904qhkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1ezpnm5</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>So the green nails! Here’s the big dump and all the angles! And the inspiration at the end.</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezpnm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1ezovbm</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>I’m proposing this year and my girlfriend’s ring finger nail needs help!</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezovbm/im_proposing_this_year_and_my_girlfriends_ring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1ezqtma</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Not my best set, but I think I might love marble matte now…</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezqtma</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1ezqtab</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>First attempt at cat eye polish!</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ddtpf3hwxhkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1ezqors</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t xml:space="preserve">re did this set to look a bit more uniform </t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggsjm9oxwhkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1ezq7ls</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>what do you guys think</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwjxb7q8thkd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1ezplin</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Gel overlay on natural nails</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezplin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1ezoqld</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Need help with fake nails</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezoqld/need_help_with_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1ezok8s</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>🥰🥰</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lt3mzt8jghkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1eznwwi</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Is there any way to get the sticky tabs off the back of this fake nail?</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dnip18zlbhkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1eznvi9</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dragonfly crocodile nails! </t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fxdj0hybbhkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1eznub8</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Client freestyle from today. All she requested was a little 3D froggy and I feel like she turned out adorable 🥹</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eznub8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1eznp12</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Builder gel removal help</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eznp12/builder_gel_removal_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1eznlca</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yeah I’m early </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aycbmrk79hkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1ezmx4o</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t xml:space="preserve">need some advice </t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezmx4o/need_some_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1ezmu6y</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Am I being too picky? Or is this acrylic set too thick?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezmu6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1ezmsv7</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted French tips with nail polish </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezmsv7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1ezmr80</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Simple First Set</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezmr80</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1ezmnry</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am nail dumping, it’s been over a year since I was on reddit. </t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezmnry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1ezml09</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>I despise pink, so I rolled into 35 with the longest, pinkest set I could handle.</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8fdwob6p1hkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1ezmj20</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Hey puddin</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3mxc86a1hkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1ezmhe0</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Last years SpOoKy set</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/junbikax0hkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1ezl8yt</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Polygel at home</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iedjcf1hrgkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1ezli6k</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love when my clients wants charms! </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vil065sftgkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1ezlfde</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>gilded</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezlfde</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1ezkt59</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>what nail shape best fits my nails?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv73ihh8ogkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1ezjlac</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing nails- need advise </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezjlac</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1ezka7l</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>not sure if i like them</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc44akrbkgkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1ezioy4</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Went classic this time 😇</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezioy4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1ezh4os</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Recovering nail-biter. How long will this indentation stick around for?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezh4os</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1ezgzxu</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>I am loving Gel X</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nb5pvctcwfkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1eyxhk3</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Nail tech removed my acrylics very harshly, I now have nail pain and want to heal my nails</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8078mfdasakd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1eyv3ml</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I cut two separate press on nails, glue them together before gluing them into my short toe thumbs? </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eyv3ml/can_i_cut_two_separate_press_on_nails_glue_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1eyrwam</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>how to achieve french nails</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eyrwam/how_to_achieve_french_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1ezhbyn</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Are these nails too short for press on nails?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypnq4pwsyfkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1ezhqzf</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Short stubby fingers on small hands </t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2fq57iu1gkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1ezhk3t</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Loving my new set</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezhk3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1ezhb70</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>A beautiful reflective design 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4ocuiknyfkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1ezecua</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Important Notice: Issues with Light Elegance Gen 3 Dot Lamps </t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.ipetitions.com/petition/recall-light-elegance-gen-3-dot-lamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1ezfspk</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Anyone have experience with madam glam?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezfspk/anyone_have_experience_with_madam_glam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1ezfp6s</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>seashell french tip nails !!</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/910ld26wmfkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1eyrn1e</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Office appropriate nails</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1eyrn1e/office_appropriate_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1ezfd10</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Half way, I just love it</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knqa0rajkfkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1ezf6g8</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Buying nail set with UV lamp from amazon</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezf6g8/buying_nail_set_with_uv_lamp_from_amazon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1ezev8o</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Sparkle Sparkle</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezev8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1ezdwbh</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Black &amp; Silver - a winning combo 🖤🩶</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3azptibt9fkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1ezdjyl</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Why the heck are my press-ons losing shape after a few days?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ezdjyl/why_the_heck_are_my_pressons_losing_shape_after_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1ezc1r6</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got to love a fresh set </t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezc1r6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1ezbcbk</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Playing with blooming gel 🐍 🐆 </t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1edbncbpekd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1ezbb87</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Pretty in pink :) The first and only time I've ever had my nails done :)</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nm9z0styoekd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1ez9v2f</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>how would you caption these?✨🧿</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez9v2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1ez9eqd</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>ILNP - VIP</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez9eqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1ez8rpx</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>shape help?</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/081unoaoydkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1ez88xw</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>End of summer fruity picnic vibes 🍒🍓</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6o6q9bjsdkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1ez7ga3</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0hpagfiidkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1f006yg</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve never been so happy to pay for shipping! </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8jetpwhkkkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1ezzj1s</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>How Is this set? ( went to a different place this time)</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezzj1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1ezzh3n</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>🌬️ Ka Like A Wind 💨 by Great Lakes Lacquer</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/ic6i3EZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1ezzdv6</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kali Goddess of Destruction </t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4jorovmaakkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1ezzb3n</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Plain and simple nail art </t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezzb3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ezxr86</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Holo Taco dupe?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezxr86/holo_taco_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ezxq50</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>LynB The Sticker (neon jellies) opinions.</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezxq50/lynb_the_sticker_neon_jellies_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ezx6bh</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Looking for Magnetic Polish Recommendations</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eusrfdzkkjkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1eztrd3</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>True pearl effect??</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dv8nl76nikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1eztjvx</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Sweet Pea, and a Dog Tax</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eztjvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1eztit4</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Sassy Sauce- Cockadoodle Doom</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eztit4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1ezss3l</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque Colors: Mango jelly is sold out; Me: we have mango jelly at home </t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezss3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ezspws</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> {PR} Sassy Sauce | Polish Pick Up - Simply Shreeeik</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezspws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ezse42</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Joie de Vivre Lurid Lacquer </t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8rd8k0ixaikd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ezrw5k</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are we feeling the red? I’m still not sure I’m loving them. </t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezrw5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ezrasr</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>What shape should I do?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezrasr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ezqom0</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Canadian Laqueristas, where the heck do you get your polish from?</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezqom0/canadian_laqueristas_where_the_heck_do_you_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ezqmp8</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t xml:space="preserve">this polish made me like magnetics </t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezqmp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ezqce0</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Non magnetic ILNP power surge dupe?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezqce0/non_magnetic_ilnp_power_surge_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ezps39</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Heartless wench</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezps39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1ezplqv</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Advice with Phoenix</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezplqv/advice_with_phoenix/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1ezolyi</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Not a fan of this topper, or at least I don't know how to use it to make it look nice. But Shaggy helped me feel better about it ❤️</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezolyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1eznzgl</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Resizing stamper! </t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cft8ji4chkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1ezn3gt</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail break </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezn3gt/nail_break/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1ezmm4y</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Plant Aunt</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezmm4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1ezmljp</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Bees Knees, Where Am I? 🫥</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugv2ez0n1hkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1ezmbvp</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>PPU Damage :-(</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck0a09erzgkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1ezm0li</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brat-adjacent summer </t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fs5g2ceexgkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1ez6zgt</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>What are the names for equipment and technique in this video?</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ez6zgt/what_are_the_names_for_equipment_and_technique_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1ezl2kq</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>PSA: Surprise restock of Clionadh Psilocybin!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4z61x35qgkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1ezl1ak</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>🥴🍏⭕️</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezl1ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1ezkpvl</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>UPDATE: Holo Taco’s Mixed Emotions Collection</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iov9nqzjngkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1ezkj8a</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Battle of the Boxes is STUNNING 💚🩵🖤</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezkj8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1ezkh2x</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>What's in a bottle?</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezkh2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1ezkcwn</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>I’m so excited for fall I did Pumpkin spice nails!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezkcwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1ezkcou</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>first time trying regular polish over builder gel 🦄</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ag572vtkgkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1ezk10t</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>prugly greens have me in a chokehold 🐍</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82bdxjbfigkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1ezjzzv</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>*Two days* without polish and this happens 😭</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnaq8wj7igkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1ezjy9y</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>beach/ocean manicure inspiration needed 🌊</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezjy9y/beachocean_manicure_inspiration_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1ezjj1w</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Cirque Colors: Morningtide and Rosewater Jellies</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezjj1w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1ezja5w</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Lumen Mysteries</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezja5w/lumen_mysteries/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1ezis70</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ah the joys of living in Canada </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4iql8z99gkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1ezirei</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Help needed!!!</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56fv0rp39gkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1ezilme</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Hello, what type of nails are these</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezilme</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1ezia7o</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>I'm not usually a red fan (on me) but I'm really enjoying this shade Fall Colorpass</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezia7o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1ezgkyw</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I can't get over how shiny the holographics are. </t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o51ggytatfkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1ezgklh</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>📝Lined Paper📝</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezgklh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1ezg7tq</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>My friends and I decorated our natural nails at a nail salon for our graduation.</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekk4opblqfkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1ezg5n2</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Yet another random object around my house that my nails match to❄️</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezg5n2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1ezg4c5</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>PSA for those that are planning on getting IKEA Helmers</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezg4c5/psa_for_those_that_are_planning_on_getting_ikea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1ezev0r</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Essie - Crochet Away</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8g4yv2zxgfkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1ezekus</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Cracked - Disco Poltergeist</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezekus</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1ezeef2</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Important Notice: Issues with Light Elegance Gen 3 Dot Lamps </t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezeef2/important_notice_issues_with_light_elegance_gen_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1ezdwrh</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">help identifying polish? </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6rpy9zw9fkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1ezcvos</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still have to wipe with a tip on? </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezcvos/still_have_to_wipe_with_a_tip_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1ezcbh1</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Mooncat price increase?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ezcbh1/mooncat_price_increase/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1ezcbay</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Ectoplasmic EdM: The Arrival</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezcbay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1ezc6l8</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>The glow is so good!! ✨</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezc6l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1eza5au</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>“Boom Chacalaca” from Bluebird Lacquer</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8lzsl4udekd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1ez9k24</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>ILNP - VIP</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez9k24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1ez7ooa</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why are drive thru lights on point for holos? </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ez7ooa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1ezw84d</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with my new Hello Kitty nails :) </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v24qigwoajkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1ezusdg</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Feelin green🌵</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/linmpulnwikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1ezurgi</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Press ons I made 🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezurgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1ezuau5</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Matt finish</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezuau5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1ezts0f</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My most recent nails </t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezts0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1ezrqvi</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>New to nail art + officially obsessed</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezrqvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1ezrenr</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>animal print</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/irnvh9oo2ikd1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1ezquvu</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Sticking press ons onto stand that isn’t putty</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ezquvu/sticking_press_ons_onto_stand_that_isnt_putty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1ezpah0</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">refined this set a bit </t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9j673ui8mhkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1eznx20</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snakes 🐍 </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eznx20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1eznpod</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>In love!!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eznpod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1eziea2</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Cat Eye Galaxy Nails</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eziea2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1ezhp4m</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seashell press on set I done for a friend. I’m personally obsessed. What are your thoughts? </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gbgrqzg1gkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1ezgmti</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Proposal nails ideas 💡</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ezgmti/proposal_nails_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1ezfioj</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nail art </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dgoue1nlfkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1ezefcl</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>🌟 Descubra o Novo Curso de Nail Designer! 🌟
+Pessoal, tenho uma dica incrível para vocês: um curso de design de unhas que está super acessível e é extremamente completo! 🎨💅 Se você está pensando em aprimorar suas habilidades ou até mesmo começar do zero, este é o curso ideal.
+👉 Preço imbatível</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://pay.kiwify.com.br/I3oGO2S?afid=Xuww0k6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1ezcx26</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail art goofing </t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezcx26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1ez8k5t</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Got my nails professionally done for the first time in years!</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt9a8ooawdkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Aug 25 08:08:44 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_08_25.xlsx
+++ b/data/2024_08_25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1128"/>
+  <dimension ref="A1:C1308"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19611,6 +19611,3066 @@
         </is>
       </c>
     </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1f0r15n</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>The most recent one</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lmkbakzykrkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1f0qc1t</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>I'm really loving almond shaped nails. Any tips for keeping everything even?</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aafqp1dybrkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1f0qalu</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Creating pinkie nails out of thin air. Not perfect, but its something</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/38jyp08gbrkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1f0pzie</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Cheap press ons I did with gel base+top coat</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0pzie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1f0nt85</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Got upset at how bad the salon did on my last manicure, so I learned how to work with dip powder</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0nt85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1f0n1lx</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Cheap red press ons I finessed</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0n1lx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1f0parw</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Very classy, very demure, very cutesy</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0parw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1f0pa8i</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">latest set </t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wucecec1zqkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1f0olnd</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I doing something wrong? </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0olnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1f0nmka</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - Blessed With Beauty and Grace</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0nmka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1f0nal6</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>new nails (gel polish, natural)</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0nal6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1f0n2mb</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Got a new set on!!🤗</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0n2mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1f0mzl8</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Kid’s nails</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0mzl8/kids_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1f0n04v</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m loving these press ons i found at Marshall’s </t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56l3upyy9qkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1f0melz</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Why do my nails look like this… they are angled up</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0melz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1f0lmh7</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>How do I fix the scratches on my nails?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0lmh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1f0klpj</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Has anyone else had issues with the le mini macaron kits?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0klpj/has_anyone_else_had_issues_with_the_le_mini/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1f0mil4</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finally jumping on the white chrome wagon and I cant believe it took this long. </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96l3hz025qkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1f0m0e9</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>My friend snapped with these XL hibiscus themed set🌺🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0m0e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1f0ltnn</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>saw another redditor using their cat as a prop and had to join the party</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0ltnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1f0lee8</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Collection </t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snyr25bbupkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1f0l5da</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>In space no one can hear your nails click</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0l5da</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1f0kdy8</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Swirly pearl nails 💅</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2twtlmmkpkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1f0iswp</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Went slightly basic with these…</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0iswp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1f0jy5v</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Work friendly korean manicure </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4u2do3igpkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1f0j76l</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Cinnamoroll Press Ons I Made!</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0j76l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1f0j4b4</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Did my nails for my engagement photoshoot!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0j4b4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1f0ixnf</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>if I want "tips" does it ~have~ to be acrylic?</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0ixnf/if_i_want_tips_does_it_have_to_be_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1f0iwqm</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>I’ve recently been doing my own Gel X nails &amp; I’m finally becoming more comfortable doing nail art. I’ve wanted these tomato nails for months 🍅</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0iwqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1f0idqk</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>So sad they’re gone 😫</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0idqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1f0hyv2</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>My Nail artist did such a great job!!!</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jug8jcd7zokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1f0htse</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>DIY nails</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm9c7gl1yokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1f0hrf7</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips for appling KBShimmer cat eye (non-gel) nail polish? (Love at First Frost) </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10xcrajaxokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1f0gonu</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Builder gel suddenly lifting and peeling off too soon?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0gonu/builder_gel_suddenly_lifting_and_peeling_off_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1f0hki9</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Color Match Help</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm9g3auvvokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1f0gzh5</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>nail tech took off some of my nail</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dx05l9ayqokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1f0h3fw</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>I never thought bowling would be so harsh on nails 😭</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0h3fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1f0gzrn</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>first time doing my nails!! every time i look at em it makes me so happy i love them! (im a guy)</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5t76l8seqokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1f0glp0</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am wearing The Instant Mani holding another The Instant Mani. </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufsucjqqnokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1f0fg3a</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these press on nails too large? Advice please! </t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0fg3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1f0gjmt</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First mani! </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0gjmt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1f0ftrw</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Questions abt fake nails</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0ftrw/questions_abt_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1f0fj2h</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for BIAB brand recommendations </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0fj2h/looking_for_biab_brand_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1f0fal3</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Manucurist green flash?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0fal3/manucurist_green_flash/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1f0f81d</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts? </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/red7ibzfcokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1f0eqrm</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>New nails!!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0eqrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1f0emsu</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Which ones for my bday</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0emsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1f0elxd</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Sassy Sauce | Giggle Juice </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0elxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1f0ellc</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Sassy Sauce | Giggle Juice </t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0ellc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1f0e7ld</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Pearl Swirl (natural nails)</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0e7ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1f0du0i</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails I did yesterday </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0du0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1f0d0qf</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Wife's Nails</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fvw0l3rrunkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1f0cr9i</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Tortoise shell nails.</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0cr9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1eztbsb</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>The nails I haven’t dumped. Some of my more subtle and not so awesome sets.</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eztbsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1f0cjir</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Gold flake ✨</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0cjir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1ezu553</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need Emotional Support On Nails </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ici87n6pqikd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1ezum5k</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>press ons</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezum5k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1f0cfli</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>When trying new polishes goes super well 🩵✨</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0cfli</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1f08ntm</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Press ons for nails with damage</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f08ntm/press_ons_for_nails_with_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1f0a13l</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My cousin did my nails, inspired by my aunt’s art, who has passed away after a long battle with cancer </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0qmg3mj7nkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1f0ajaf</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Going to get my nails done professionally for the first time is there a script i can use?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0ajaf/going_to_get_my_nails_done_professionally_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1f0c8j3</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Nail shape?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybx9c53monkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1f0caqe</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Very cutesy very demure</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0caqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1f0bz1n</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>they kind of look like cornflakes in milk… 😃</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vk9owkzjmnkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1f0byq5</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Something new</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0byq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1f0b6ev</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set </t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3tx72gegnkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1f0awo9</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/modgg97aenkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1f0aojs</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>What’s going on with my nails here? Dry/cracking</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f0aojs/whats_going_on_with_my_nails_here_drycracking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1f0anrx</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvxoiy6dcnkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1f0a74j</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Been over a year since I marbled my nails</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0a74j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1f09z06</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Sparkly space princess set ✨</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sids3bg27nkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1f09vgz</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Blue white and gold</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f09vgz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1f09o2n</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>First Time getting regular polish. Are these really bad or normal for this type of polish?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kusunvsn4nkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1f09o1i</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">End of summer mani </t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq03n51n4nkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1f08ts3</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First *simple* nail art attempt </t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72zrws44ymkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1f06m4k</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Glue that won't harm moms nails</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f06m4k/glue_that_wont_harm_moms_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1f08nrj</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Cuticle oil recommendations?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f08nrj/cuticle_oil_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1f08e2h</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Sparkles and me forever</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st1akp1uumkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1f08cyd</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Learning to love polish!</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbo31x0jumkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1f0863z</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>I understand this might not be everyone’s favourite style or their cup of tea but I just wanted to show them off</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0863z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1f082fc</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Rojo</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk5ydgubsmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1f07sdl</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry-picked sweetness 🍒 </t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqsvycz4qmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1f07qwr</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel cloud manicure on natural nails. I’m still learning what products work best for me, definitely room for improvement. </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f07qwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1f07qpb</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t decide if I like </t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkxc2rwspmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1f07l8x</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>I don’t think we’re in Kansas anymore</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw05zp2nomkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1f075l4</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dying over my last summer set </t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f075l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1f06c85</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Stray Kids Nails Part 1</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f06c85</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1f06bid</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>🦋</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pczjp66pemkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1f06105</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question About Shapes </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f06105/question_about_shapes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1f05u1f</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Is there a way to refill these? I love the convenience but find it too wasteful to purchase again</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/by9bhdrnamkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1f05i8c</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">meltin' </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f05i8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1f058id</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Press ons for weak nails</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f058id/press_ons_for_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1f055v9</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got my nails done professionally for the first time ever </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f055v9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1f04rxs</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Press On Nails</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://v.lemon8-app.com/s/AmyRkwjspR</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1f04d2d</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Felt nostalgic for Saturday morning cartoons and bowling alley carpet. </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f04d2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1f04apa</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Jojo’s Bizarre Adventure nails!</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f04apa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1f02iub</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Uneven nail edges</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cg3jv8wfelkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1f028xx</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Can I take nail varnish off my toes with biab/gel polish on my finger nails?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1f028xx/can_i_take_nail_varnish_off_my_toes_with_biabgel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1eztdjz</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>my nails vs what i showed my nail tech! (inspo: riley jane on pinterest)</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1eztdjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ezvtaj</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Nails done in Shinjuku JPN</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ezvtaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1f0rd42</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>My nails natural</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dgccufwbprkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1f0qv1s</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Very cutesy, very demure ✨</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0qv1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1f0quy7</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Very cutesy, very demure ✨</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0quy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1f0qq9a</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> comparisons of Mooncat's Mermaid Bait, Petals for a Narcissist, and Ghosts of Hecate?</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0qq9a/comparisons_of_mooncats_mermaid_bait_petals_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1f0q3hu</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Demure fall? No, brat summer forever!</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uw4ekvvy8rkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1f0nnlo</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers - Blessed With Beauty and Grace</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0nnlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1f0nmoi</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Base and top coats</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0nmoi/base_and_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1f0nb9k</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Y'all... did I just get a magnetic polish to actually *magnetize*??</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rfipne5dqkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1f0n4zx</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The camera will never capture how pretty this one is </t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0n4zx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1f0mh3v</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>elden ring lacquer !!!!</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0mh3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1f0mb1y</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how do i use this cuticle cutter? </t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/px3qyh113qkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1f0m8gc</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>sand viper by mooncat 🍦</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ng42739b2qkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1f0m60w</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holo Taco Wicked Potion vs Lost in the Woods </t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0m60w/holo_taco_wicked_potion_vs_lost_in_the_woods/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1f0m0pu</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Vintage 2001 chrome</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0m0pu/vintage_2001_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1f0luy0</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite dark/ jewel-toned polishes? </t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0luy0/favorite_dark_jeweltoned_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1f0lrxi</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I save this? </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0lrxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1f0kpr9</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>The many colors of Phoenix Indie Pelvic Sorcery</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdd4yrdpnpkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1f0khwt</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>questions about nail scrubbers</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihmbqjjnlpkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1f0jb2x</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>everyone was right about ILNP flower child</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0jb2x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1f0i53r</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL Get Lobstered &amp; Lyn B. Trouvaille </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0i53r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1f0hno2</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>I went to the beauty salon to pamper my natural nails, I loved them</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pt3l97slwokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1f0hk44</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>How many of ya’ll take a photo of your latest gorgeous manicure to post it here only to delete it because the camera can never capture the true beauty of the polish???</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0hk44</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1f0gh77</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Working on application </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0gh77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1f0gh33</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>How to add length W/O damaging nail bed!?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0gh33/how_to_add_length_wo_damaging_nail_bed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1f0ggok</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Didn’t realize this bracelet I bought matched until I got home!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85lrv22mmokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1f0gccv</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>A Mani with two PPU polishes</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0gccv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1f08nrs</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Baby's first PPU</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6450boxwmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1f0fjda</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>HEMA concerns</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0fjda/hema_concerns/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1f0feke</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>The manicure vs. the inspo! I was too lazy to clean them up perfectly, but I still love it 💙💚 I have a camping trip coming up so after this, it's time to chop! 🥲</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0feke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1f0f97x</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Glisten and Glow vs Seche Vite</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0f97x/glisten_and_glow_vs_seche_vite/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1f0es2p</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>It rained here yesterday, so I did Autumn nails.</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0es2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1f0ejma</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{PR} Sassy Sauce | Giggle Juice </t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0ejma</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1f0efgn</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Memorial nails 🐈</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0efgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1f0ebbt</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Look at this adorable baby polish 🤩</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d3grk655okd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1f0drke</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“Sour Apple Rings” from Atomic Polish. Letters are fake. Brat girl summer engaged. </t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0drke</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1f0d10n</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amazing but not as advertised </t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0d10n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1f0czhu</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Mooncat dupes?</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0czhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1f0cynb</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>First time trying ILNP!!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1k3s8kbunkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1f0co74</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Show me your Cliondagh Dark and Stormy nail pic, please!</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0co74/show_me_your_cliondagh_dark_and_stormy_nail_pic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1f0cdo4</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Ducking tax, sound on... excuse my tips</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0f3ug04rpnkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1f0cdl8</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Favorite transition season colors?</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kq4fpnqqpnkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1f0bvuj</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Turquoise creme + floral stickers 🌸</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/bBDXyo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1f0blut</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>fresh mani on my short nails !</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3zqxdspjnkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1f0bjmg</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I ordered a nail strengthener, but now I saw that it has formaldehyde </t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f0bjmg/i_ordered_a_nail_strengthener_but_now_i_saw_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1f0agiq</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Does it fit my skintone?</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3h2uuretankd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1f09x1x</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Bye-bye Summer</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f09x1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1f09vlf</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍸 Jackie Daytona: Regular Human Bartender 🏐 by LynB Designs 🧛🏻‍♀️ </t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hnz9j9856nkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1f09ujg</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>This look?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mgt5mr26nkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1f09qcl</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Lovey Dovey nails for my partner and I's anniversary &lt;3</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5rvvun05nkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1f09cix</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thanks to the advice from this sub, I finally had a mani last more than 24 hours without a single chip! I feel invincible </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f09cix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1f08sjk</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Ether Dragon Jelly Sandwich</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13sa5eosxmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1f0864q</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Orly Star Fire over black base + shimmer</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jgk6tu4tmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1f07vfk</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Black coffe nail polish: what brand could I choose</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f07vfk/black_coffe_nail_polish_what_brand_could_i_choose/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1f07rq3</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If they must be short, let them be bold! </t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d430o0r0qmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1f07r63</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using a makeup sponge </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t6b4yjuvpmkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1f07qs5</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Hecate - Femme Fatale</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/usm4xjftpmkd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1f07pb0</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>So, does anyone actually use a full bottle of top coat?</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1f07pb0/so_does_anyone_actually_use_a_full_bottle_of_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1f07g0b</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Matte and glossy</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f07g0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1f07bxi</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Essie - Island Hopping</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4t4642pmmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1f058o1</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>The best long-lasting drugstore polish 💅</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kpp1w5hm5mkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1f04drf</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I go back to the salon for this </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9xxfzb2ylkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1f03x4z</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>First ever attempt at nailart 🧿 not perfect, but happy with it</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwxxii7ltlkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1f02ogl</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Almost Springtime makes me want to bring out the bright colours! 💖</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f02ogl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1f0jvo0</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Help with new set</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0jvo0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1f0jmwr</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Matching sets</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdfr9rwmdpkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1f0j6q1</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Cinnamoroll Press Ons I Made!</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0j6q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1f0fhbc</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>I rarely see this green anymore</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0fhbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1f0f9so</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>My one week old nails</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vkdiicfucokd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1f0d9a2</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>“Sisters, not twins” 😂 art by me</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uaujdvlnwnkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1f0ciqr</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love this set so much </t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0ciqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1f0c7hs</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm back to pink </t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsnwxzzdonkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1f0c1ix</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Y2K Gothic Inspired Kuromi Press Ons I Made!</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f0c1ix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1f0boru</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Anyone into these dragon nails I did a while back? Was testing out some new techniques 🐲💚</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/frp8mafcknkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1f09wfk</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Blue white and gold</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f09wfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1f06zj3</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>I did it with the eyeshadow and glitter nailpolish</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrjovt71kmkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1f03gh0</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>A little something I did with the Orly 'Melting Point' set ✨</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f03gh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1f0350e</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Is it possible to do nail art with chrome powder and regular polish, but only for small details?</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1f0350e/is_it_possible_to_do_nail_art_with_chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1f02x1m</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very first attempt! </t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f02x1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1f00q8x</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chakra press on set. Would you wear these? </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mbbu577grkkd1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1f00fbb</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>some inspo with ocean🌊</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1f00fbb</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>